<commit_message>
Deployed 211e2f0 with MkDocs version: 1.6.1
</commit_message>
<xml_diff>
--- a/downloads/data/bnr-cvd-2023-table1.xlsx
+++ b/downloads/data/bnr-cvd-2023-table1.xlsx
@@ -13,7 +13,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" count="53" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" count="54" uniqueCount="25">
   <si>
     <t>CVD Event Type (AMI=2, Stroke=1)</t>
   </si>
@@ -86,6 +86,9 @@
   <si>
     <t xml:space="preserve">  Total</t>
   </si>
+  <si>
+    <t>Prepared by Ian Hambleton on 2025-11-19, for the Barbados National Registry</t>
+  </si>
 </sst>
 </file>
 
@@ -8966,7 +8969,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J21"/>
+  <dimension ref="A1:J22"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -9618,6 +9621,11 @@
         <v>16306</v>
       </c>
     </row>
+    <row r="22">
+      <c r="A22" t="s">
+        <v>24</v>
+      </c>
+    </row>
   </sheetData>
   <mergeCells count="7">
     <mergeCell ref="B1:J1"/>

</xml_diff>